<commit_message>
Struktur für COB hergestellt, sowie grobe GUI gebaut und Highscoreliste integriert
</commit_message>
<xml_diff>
--- a/AktienEngine.View/bin/Debug/net8.0-windows/TimeLogger.xlsx
+++ b/AktienEngine.View/bin/Debug/net8.0-windows/TimeLogger.xlsx
@@ -28,37 +28,16 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:si>
-    <x:t>Programmierung des Launchers fertiggestellt und Klasse zur Zeitplanung erstellt</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Programmierung des Launchers, Verbinden von VM zur V</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Grundgerüst und Aufbau der MVVM-Struktur fertiggstellt</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Projektplanung und Grundgerüst erstellt</x:t>
-  </x:si>
-  <x:si>
     <x:t>Arbeit</x:t>
   </x:si>
   <x:si>
-    <x:t>4</x:t>
-  </x:si>
-  <x:si>
-    <x:t>3</x:t>
-  </x:si>
-  <x:si>
-    <x:t>2</x:t>
-  </x:si>
-  <x:si>
-    <x:t>5</x:t>
+    <x:t/>
   </x:si>
   <x:si>
     <x:t>Stunden</x:t>
   </x:si>
   <x:si>
-    <x:t>01.10.2025</x:t>
+    <x:t>ClosedXML.Excel.XLCellValue[]</x:t>
   </x:si>
   <x:si>
     <x:t>Datum</x:t>
@@ -411,43 +390,43 @@
   <x:sheetData>
     <x:row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <x:c r="A1" s="0" t="s">
-        <x:v>11</x:v>
+        <x:v>4</x:v>
       </x:c>
       <x:c r="B1" s="0" t="s">
-        <x:v>9</x:v>
+        <x:v>2</x:v>
       </x:c>
       <x:c r="C1" s="0" t="s">
-        <x:v>4</x:v>
+        <x:v>0</x:v>
       </x:c>
     </x:row>
     <x:row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <x:c r="A2" s="0" t="s">
-        <x:v>10</x:v>
+        <x:v>3</x:v>
       </x:c>
       <x:c r="B2" s="0" t="s">
-        <x:v>8</x:v>
+        <x:v>1</x:v>
       </x:c>
       <x:c r="C2" s="0" t="s">
-        <x:v>3</x:v>
+        <x:v>1</x:v>
       </x:c>
     </x:row>
     <x:row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <x:c r="A3" s="0" t="s">
-        <x:v>10</x:v>
+        <x:v>3</x:v>
       </x:c>
       <x:c r="B3" s="0" t="s">
-        <x:v>7</x:v>
+        <x:v>1</x:v>
       </x:c>
       <x:c r="C3" s="0" t="s">
-        <x:v>2</x:v>
+        <x:v>1</x:v>
       </x:c>
     </x:row>
     <x:row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <x:c r="A4" s="0" t="s">
-        <x:v>10</x:v>
+        <x:v>3</x:v>
       </x:c>
       <x:c r="B4" s="0" t="s">
-        <x:v>6</x:v>
+        <x:v>1</x:v>
       </x:c>
       <x:c r="C4" s="0" t="s">
         <x:v>1</x:v>
@@ -455,13 +434,13 @@
     </x:row>
     <x:row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <x:c r="A5" s="0" t="s">
-        <x:v>10</x:v>
+        <x:v>3</x:v>
       </x:c>
       <x:c r="B5" s="0" t="s">
-        <x:v>5</x:v>
+        <x:v>1</x:v>
       </x:c>
       <x:c r="C5" s="0" t="s">
-        <x:v>0</x:v>
+        <x:v>1</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>